<commit_message>
added Document SI version
added Bagan Akun and IFG (Input Form Guide)
</commit_message>
<xml_diff>
--- a/Dokumen-si/IFG-Penerimaan dan Pengeluaran.xlsx
+++ b/Dokumen-si/IFG-Penerimaan dan Pengeluaran.xlsx
@@ -957,12 +957,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -976,6 +970,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1294,8 +1294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -1304,7 +1304,7 @@
     <col min="2" max="2" width="35.5703125" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.140625" style="23" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" style="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.140625" style="47" customWidth="1"/>
     <col min="8" max="8" width="29.140625" style="42" bestFit="1" customWidth="1"/>
@@ -1320,21 +1320,21 @@
     <row r="2" spans="1:17" x14ac:dyDescent="0.4">
       <c r="E2" s="7"/>
       <c r="F2" s="8"/>
-      <c r="G2" s="91" t="s">
+      <c r="G2" s="104" t="s">
         <v>72</v>
       </c>
-      <c r="H2" s="91"/>
-      <c r="I2" s="92" t="s">
+      <c r="H2" s="104"/>
+      <c r="I2" s="105" t="s">
         <v>93</v>
       </c>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
-      <c r="Q2" s="105" t="s">
+      <c r="J2" s="105"/>
+      <c r="K2" s="105"/>
+      <c r="L2" s="105"/>
+      <c r="M2" s="105"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="105"/>
+      <c r="Q2" s="103" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1355,7 +1355,7 @@
       <c r="H3" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="Q3" s="100"/>
+      <c r="Q3" s="98"/>
     </row>
     <row r="4" spans="1:17" s="37" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="33" t="s">
@@ -1367,11 +1367,11 @@
       <c r="E4" s="36"/>
       <c r="G4" s="49"/>
       <c r="H4" s="44"/>
-      <c r="I4" s="93"/>
-      <c r="J4" s="93"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
-      <c r="Q4" s="101"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="Q4" s="99"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B5" s="64" t="s">
@@ -1381,11 +1381,11 @@
       <c r="D5" s="66"/>
       <c r="E5" s="67"/>
       <c r="F5" s="68"/>
-      <c r="I5" s="94"/>
-      <c r="J5" s="94"/>
-      <c r="K5" s="94"/>
-      <c r="L5" s="94"/>
-      <c r="Q5" s="102" t="s">
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
+      <c r="Q5" s="100" t="s">
         <v>91</v>
       </c>
     </row>
@@ -1399,18 +1399,18 @@
       <c r="F6" s="70"/>
       <c r="G6" s="55"/>
       <c r="H6" s="61"/>
-      <c r="I6" s="94"/>
-      <c r="J6" s="94"/>
-      <c r="K6" s="94"/>
-      <c r="L6" s="94"/>
-      <c r="Q6" s="102"/>
+      <c r="I6" s="92"/>
+      <c r="J6" s="92"/>
+      <c r="K6" s="92"/>
+      <c r="L6" s="92"/>
+      <c r="Q6" s="100"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B7" s="69"/>
       <c r="C7" s="26"/>
       <c r="D7" s="56"/>
       <c r="E7" s="11">
-        <v>401</v>
+        <v>1111</v>
       </c>
       <c r="F7" s="71" t="s">
         <v>4</v>
@@ -1421,19 +1421,19 @@
       <c r="H7" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J7" s="98" t="s">
+      <c r="I7" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="K7" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L7" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q7" s="102">
+      <c r="K7" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L7" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q7" s="100">
         <v>1</v>
       </c>
     </row>
@@ -1442,30 +1442,30 @@
       <c r="C8" s="26"/>
       <c r="D8" s="57"/>
       <c r="E8" s="58">
-        <v>402</v>
+        <v>1112</v>
       </c>
       <c r="F8" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="97" t="s">
+      <c r="G8" s="95" t="s">
         <v>66</v>
       </c>
       <c r="H8" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J8" s="98" t="s">
+      <c r="I8" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="K8" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L8" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q8" s="102">
+      <c r="K8" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q8" s="100">
         <v>1</v>
       </c>
     </row>
@@ -1479,39 +1479,39 @@
       <c r="F9" s="70"/>
       <c r="G9" s="55"/>
       <c r="H9" s="61"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
-      <c r="Q9" s="102"/>
+      <c r="I9" s="92"/>
+      <c r="J9" s="92"/>
+      <c r="K9" s="92"/>
+      <c r="L9" s="92"/>
+      <c r="Q9" s="100"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B10" s="69"/>
       <c r="C10" s="26"/>
       <c r="D10" s="57"/>
       <c r="E10" s="58">
-        <v>410</v>
+        <v>1120</v>
       </c>
       <c r="F10" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="97" t="s">
+      <c r="G10" s="95" t="s">
         <v>66</v>
       </c>
       <c r="H10" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J10" s="99"/>
-      <c r="K10" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L10" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q10" s="102">
+      <c r="I10" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" s="97"/>
+      <c r="K10" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q10" s="100">
         <v>2</v>
       </c>
     </row>
@@ -1525,41 +1525,41 @@
       <c r="F11" s="70"/>
       <c r="G11" s="55"/>
       <c r="H11" s="61"/>
-      <c r="I11" s="94"/>
+      <c r="I11" s="92"/>
       <c r="J11" s="10"/>
-      <c r="K11" s="94"/>
-      <c r="L11" s="94"/>
-      <c r="Q11" s="102"/>
+      <c r="K11" s="92"/>
+      <c r="L11" s="92"/>
+      <c r="Q11" s="100"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B12" s="69"/>
       <c r="C12" s="26"/>
       <c r="D12" s="57"/>
       <c r="E12" s="58">
-        <v>420</v>
+        <v>1130</v>
       </c>
       <c r="F12" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="97" t="s">
+      <c r="G12" s="95" t="s">
         <v>66</v>
       </c>
       <c r="H12" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="I12" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J12" s="98" t="s">
+      <c r="I12" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J12" s="96" t="s">
         <v>89</v>
       </c>
-      <c r="K12" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L12" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q12" s="102">
+      <c r="K12" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L12" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q12" s="100">
         <v>1</v>
       </c>
     </row>
@@ -1573,41 +1573,41 @@
       <c r="F13" s="70"/>
       <c r="G13" s="55"/>
       <c r="H13" s="61"/>
-      <c r="I13" s="94"/>
+      <c r="I13" s="92"/>
       <c r="J13" s="10"/>
-      <c r="K13" s="94"/>
-      <c r="L13" s="94"/>
-      <c r="Q13" s="102"/>
+      <c r="K13" s="92"/>
+      <c r="L13" s="92"/>
+      <c r="Q13" s="100"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B14" s="69"/>
       <c r="C14" s="26"/>
       <c r="D14" s="57"/>
       <c r="E14" s="58">
-        <v>430</v>
+        <v>1140</v>
       </c>
       <c r="F14" s="73" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="97" t="s">
+      <c r="G14" s="95" t="s">
         <v>66</v>
       </c>
       <c r="H14" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="I14" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J14" s="98" t="s">
+      <c r="I14" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J14" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="K14" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L14" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q14" s="102">
+      <c r="K14" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L14" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q14" s="100">
         <v>1</v>
       </c>
     </row>
@@ -1621,18 +1621,18 @@
       <c r="F15" s="70"/>
       <c r="G15" s="55"/>
       <c r="H15" s="61"/>
-      <c r="I15" s="94"/>
+      <c r="I15" s="92"/>
       <c r="J15" s="10"/>
-      <c r="K15" s="94"/>
-      <c r="L15" s="94"/>
-      <c r="Q15" s="102"/>
+      <c r="K15" s="92"/>
+      <c r="L15" s="92"/>
+      <c r="Q15" s="100"/>
     </row>
     <row r="16" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="74"/>
       <c r="C16" s="75"/>
       <c r="D16" s="57"/>
       <c r="E16" s="58">
-        <v>499</v>
+        <v>1150</v>
       </c>
       <c r="F16" s="73" t="s">
         <v>9</v>
@@ -1643,28 +1643,28 @@
       <c r="H16" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="I16" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J16" s="99"/>
-      <c r="K16" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L16" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q16" s="102">
+      <c r="I16" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16" s="97"/>
+      <c r="K16" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L16" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q16" s="100">
         <v>2</v>
       </c>
     </row>
     <row r="17" spans="2:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E17" s="7"/>
       <c r="F17" s="8"/>
-      <c r="I17" s="94"/>
+      <c r="I17" s="92"/>
       <c r="J17" s="10"/>
-      <c r="K17" s="94"/>
-      <c r="L17" s="94"/>
-      <c r="Q17" s="102"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
+      <c r="Q17" s="100"/>
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B18" s="76" t="s">
@@ -1674,11 +1674,11 @@
       <c r="D18" s="66"/>
       <c r="E18" s="67"/>
       <c r="F18" s="68"/>
-      <c r="I18" s="94"/>
+      <c r="I18" s="92"/>
       <c r="J18" s="10"/>
-      <c r="K18" s="94"/>
-      <c r="L18" s="94"/>
-      <c r="Q18" s="102"/>
+      <c r="K18" s="92"/>
+      <c r="L18" s="92"/>
+      <c r="Q18" s="100"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B19" s="69"/>
@@ -1690,18 +1690,18 @@
       <c r="F19" s="70"/>
       <c r="G19" s="55"/>
       <c r="H19" s="61"/>
-      <c r="I19" s="94"/>
+      <c r="I19" s="92"/>
       <c r="J19" s="10"/>
-      <c r="K19" s="94"/>
-      <c r="L19" s="94"/>
-      <c r="Q19" s="102"/>
+      <c r="K19" s="92"/>
+      <c r="L19" s="92"/>
+      <c r="Q19" s="100"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B20" s="69"/>
       <c r="C20" s="26"/>
       <c r="D20" s="56"/>
       <c r="E20" s="11">
-        <v>441</v>
+        <v>1261</v>
       </c>
       <c r="F20" s="71" t="s">
         <v>12</v>
@@ -1712,17 +1712,17 @@
       <c r="H20" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="I20" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J20" s="99"/>
-      <c r="K20" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L20" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q20" s="102">
+      <c r="I20" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J20" s="97"/>
+      <c r="K20" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L20" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q20" s="100">
         <v>2</v>
       </c>
     </row>
@@ -1731,7 +1731,7 @@
       <c r="C21" s="26"/>
       <c r="D21" s="56"/>
       <c r="E21" s="11">
-        <v>442</v>
+        <v>1262</v>
       </c>
       <c r="F21" s="71" t="s">
         <v>13</v>
@@ -1742,17 +1742,17 @@
       <c r="H21" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J21" s="99"/>
-      <c r="K21" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L21" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q21" s="102">
+      <c r="I21" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J21" s="97"/>
+      <c r="K21" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L21" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q21" s="100">
         <v>2</v>
       </c>
     </row>
@@ -1761,7 +1761,7 @@
       <c r="C22" s="26"/>
       <c r="D22" s="56"/>
       <c r="E22" s="11">
-        <v>443</v>
+        <v>1263</v>
       </c>
       <c r="F22" s="71" t="s">
         <v>14</v>
@@ -1772,17 +1772,17 @@
       <c r="H22" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="I22" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J22" s="99"/>
-      <c r="K22" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L22" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q22" s="102">
+      <c r="I22" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J22" s="97"/>
+      <c r="K22" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L22" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q22" s="100">
         <v>2</v>
       </c>
     </row>
@@ -1791,28 +1791,28 @@
       <c r="C23" s="26"/>
       <c r="D23" s="57"/>
       <c r="E23" s="58">
-        <v>444</v>
+        <v>1264</v>
       </c>
       <c r="F23" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="97" t="s">
+      <c r="G23" s="95" t="s">
         <v>71</v>
       </c>
       <c r="H23" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="I23" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J23" s="99"/>
-      <c r="K23" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L23" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q23" s="102">
+      <c r="I23" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J23" s="97"/>
+      <c r="K23" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L23" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q23" s="100">
         <v>2</v>
       </c>
     </row>
@@ -1826,41 +1826,41 @@
       <c r="F24" s="70"/>
       <c r="G24" s="55"/>
       <c r="H24" s="61"/>
-      <c r="I24" s="94"/>
-      <c r="J24" s="94"/>
-      <c r="K24" s="94"/>
-      <c r="L24" s="94"/>
-      <c r="Q24" s="102"/>
+      <c r="I24" s="92"/>
+      <c r="J24" s="92"/>
+      <c r="K24" s="92"/>
+      <c r="L24" s="92"/>
+      <c r="Q24" s="100"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B25" s="69"/>
       <c r="C25" s="26"/>
       <c r="D25" s="57"/>
       <c r="E25" s="58">
-        <v>450</v>
+        <v>1270</v>
       </c>
       <c r="F25" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="G25" s="97" t="s">
+      <c r="G25" s="95" t="s">
         <v>71</v>
       </c>
       <c r="H25" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="I25" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J25" s="98" t="s">
+      <c r="I25" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J25" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="K25" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L25" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q25" s="102">
+      <c r="K25" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L25" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q25" s="100">
         <v>1</v>
       </c>
     </row>
@@ -1874,18 +1874,18 @@
       <c r="F26" s="70"/>
       <c r="G26" s="55"/>
       <c r="H26" s="61"/>
-      <c r="I26" s="94"/>
-      <c r="J26" s="94"/>
-      <c r="K26" s="94"/>
-      <c r="L26" s="94"/>
-      <c r="Q26" s="102"/>
+      <c r="I26" s="92"/>
+      <c r="J26" s="92"/>
+      <c r="K26" s="92"/>
+      <c r="L26" s="92"/>
+      <c r="Q26" s="100"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B27" s="69"/>
       <c r="C27" s="26"/>
       <c r="D27" s="56"/>
       <c r="E27" s="11">
-        <v>461</v>
+        <v>1281</v>
       </c>
       <c r="F27" s="71" t="s">
         <v>19</v>
@@ -1896,19 +1896,19 @@
       <c r="H27" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="I27" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J27" s="98" t="s">
+      <c r="I27" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J27" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="K27" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L27" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q27" s="102">
+      <c r="K27" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L27" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q27" s="100">
         <v>1</v>
       </c>
     </row>
@@ -1917,7 +1917,7 @@
       <c r="C28" s="26"/>
       <c r="D28" s="56"/>
       <c r="E28" s="11">
-        <v>462</v>
+        <v>1282</v>
       </c>
       <c r="F28" s="71" t="s">
         <v>20</v>
@@ -1928,17 +1928,17 @@
       <c r="H28" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="I28" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J28" s="99"/>
-      <c r="K28" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L28" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q28" s="102">
+      <c r="I28" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J28" s="97"/>
+      <c r="K28" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L28" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q28" s="100">
         <v>2</v>
       </c>
     </row>
@@ -1947,7 +1947,7 @@
       <c r="C29" s="26"/>
       <c r="D29" s="56"/>
       <c r="E29" s="11">
-        <v>463</v>
+        <v>1283</v>
       </c>
       <c r="F29" s="71" t="s">
         <v>21</v>
@@ -1958,19 +1958,19 @@
       <c r="H29" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="I29" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J29" s="98" t="s">
+      <c r="I29" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J29" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="K29" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L29" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q29" s="102">
+      <c r="K29" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L29" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q29" s="100">
         <v>1</v>
       </c>
     </row>
@@ -1979,7 +1979,7 @@
       <c r="C30" s="26"/>
       <c r="D30" s="56"/>
       <c r="E30" s="11">
-        <v>464</v>
+        <v>1284</v>
       </c>
       <c r="F30" s="71" t="s">
         <v>22</v>
@@ -1990,19 +1990,19 @@
       <c r="H30" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="I30" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J30" s="98" t="s">
+      <c r="I30" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J30" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="K30" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L30" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q30" s="102">
+      <c r="K30" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L30" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q30" s="100">
         <v>1</v>
       </c>
     </row>
@@ -2011,7 +2011,7 @@
       <c r="C31" s="26"/>
       <c r="D31" s="56"/>
       <c r="E31" s="11">
-        <v>465</v>
+        <v>1285</v>
       </c>
       <c r="F31" s="71" t="s">
         <v>23</v>
@@ -2022,19 +2022,19 @@
       <c r="H31" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="I31" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J31" s="98" t="s">
+      <c r="I31" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J31" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="K31" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L31" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q31" s="102">
+      <c r="K31" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L31" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q31" s="100">
         <v>1</v>
       </c>
     </row>
@@ -2043,7 +2043,7 @@
       <c r="C32" s="26"/>
       <c r="D32" s="56"/>
       <c r="E32" s="11">
-        <v>466</v>
+        <v>1286</v>
       </c>
       <c r="F32" s="71" t="s">
         <v>24</v>
@@ -2054,19 +2054,19 @@
       <c r="H32" s="62" t="s">
         <v>24</v>
       </c>
-      <c r="I32" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J32" s="98" t="s">
+      <c r="I32" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J32" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="K32" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L32" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q32" s="102">
+      <c r="K32" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L32" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q32" s="100">
         <v>1</v>
       </c>
     </row>
@@ -2075,7 +2075,7 @@
       <c r="C33" s="75"/>
       <c r="D33" s="57"/>
       <c r="E33" s="58">
-        <v>467</v>
+        <v>1287</v>
       </c>
       <c r="F33" s="73" t="s">
         <v>25</v>
@@ -2086,26 +2086,26 @@
       <c r="H33" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="I33" s="98" t="s">
-        <v>76</v>
-      </c>
-      <c r="J33" s="98" t="s">
+      <c r="I33" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="J33" s="96" t="s">
         <v>77</v>
       </c>
-      <c r="K33" s="98" t="s">
-        <v>78</v>
-      </c>
-      <c r="L33" s="98" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q33" s="102">
+      <c r="K33" s="96" t="s">
+        <v>78</v>
+      </c>
+      <c r="L33" s="96" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q33" s="100">
         <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.4">
       <c r="E34" s="7"/>
       <c r="F34" s="8"/>
-      <c r="Q34" s="102"/>
+      <c r="Q34" s="100"/>
     </row>
     <row r="35" spans="1:17" s="2" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A35" s="33" t="s">
@@ -2117,7 +2117,7 @@
       <c r="E35" s="32"/>
       <c r="G35" s="50"/>
       <c r="H35" s="45"/>
-      <c r="Q35" s="103"/>
+      <c r="Q35" s="101"/>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B36" s="28" t="s">
@@ -2127,7 +2127,7 @@
       <c r="D36" s="19"/>
       <c r="E36" s="12"/>
       <c r="F36" s="13"/>
-      <c r="Q36" s="102" t="s">
+      <c r="Q36" s="100" t="s">
         <v>92</v>
       </c>
     </row>
@@ -2136,7 +2136,7 @@
       <c r="C37" s="26"/>
       <c r="D37" s="20"/>
       <c r="E37" s="11">
-        <v>102</v>
+        <v>2110</v>
       </c>
       <c r="F37" s="79" t="s">
         <v>30</v>
@@ -2150,7 +2150,7 @@
       <c r="I37" t="s">
         <v>76</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J37" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K37" t="s">
@@ -2171,7 +2171,7 @@
       <c r="P37" t="s">
         <v>86</v>
       </c>
-      <c r="Q37" s="102">
+      <c r="Q37" s="100">
         <v>1</v>
       </c>
     </row>
@@ -2180,7 +2180,7 @@
       <c r="C38" s="26"/>
       <c r="D38" s="20"/>
       <c r="E38" s="11">
-        <v>112</v>
+        <v>2120</v>
       </c>
       <c r="F38" s="79" t="s">
         <v>29</v>
@@ -2194,7 +2194,7 @@
       <c r="I38" t="s">
         <v>76</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J38" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K38" t="s">
@@ -2215,7 +2215,7 @@
       <c r="P38" t="s">
         <v>86</v>
       </c>
-      <c r="Q38" s="102">
+      <c r="Q38" s="100">
         <v>1</v>
       </c>
     </row>
@@ -2224,7 +2224,7 @@
       <c r="C39" s="27"/>
       <c r="D39" s="21"/>
       <c r="E39" s="15">
-        <v>117</v>
+        <v>2130</v>
       </c>
       <c r="F39" s="80" t="s">
         <v>31</v>
@@ -2238,10 +2238,10 @@
       <c r="I39" t="s">
         <v>76</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J39" s="93" t="s">
         <v>80</v>
       </c>
-      <c r="K39" s="95" t="s">
+      <c r="K39" s="93" t="s">
         <v>87</v>
       </c>
       <c r="L39" s="2"/>
@@ -2257,14 +2257,14 @@
       <c r="P39" t="s">
         <v>86</v>
       </c>
-      <c r="Q39" s="102">
+      <c r="Q39" s="100">
         <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E40" s="7"/>
       <c r="F40" s="8"/>
-      <c r="Q40" s="102"/>
+      <c r="Q40" s="100"/>
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B41" s="28" t="s">
@@ -2274,7 +2274,7 @@
       <c r="D41" s="19"/>
       <c r="E41" s="12"/>
       <c r="F41" s="13"/>
-      <c r="Q41" s="102"/>
+      <c r="Q41" s="100"/>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B42" s="16"/>
@@ -2284,7 +2284,7 @@
       <c r="D42" s="20"/>
       <c r="E42" s="9"/>
       <c r="F42" s="14"/>
-      <c r="Q42" s="102"/>
+      <c r="Q42" s="100"/>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B43" s="16"/>
@@ -2294,14 +2294,14 @@
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="14"/>
-      <c r="Q43" s="102"/>
+      <c r="Q43" s="100"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B44" s="16"/>
       <c r="C44" s="26"/>
       <c r="D44" s="20"/>
       <c r="E44" s="11">
-        <v>501</v>
+        <v>22111</v>
       </c>
       <c r="F44" s="79" t="s">
         <v>34</v>
@@ -2315,7 +2315,7 @@
       <c r="I44" t="s">
         <v>76</v>
       </c>
-      <c r="J44" s="95" t="s">
+      <c r="J44" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K44" t="s">
@@ -2324,7 +2324,7 @@
       <c r="L44" t="s">
         <v>79</v>
       </c>
-      <c r="Q44" s="102">
+      <c r="Q44" s="100">
         <v>2</v>
       </c>
     </row>
@@ -2347,7 +2347,7 @@
       <c r="I45" t="s">
         <v>76</v>
       </c>
-      <c r="J45" s="95" t="s">
+      <c r="J45" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K45" t="s">
@@ -2356,7 +2356,7 @@
       <c r="L45" t="s">
         <v>79</v>
       </c>
-      <c r="Q45" s="102">
+      <c r="Q45" s="100">
         <v>2</v>
       </c>
     </row>
@@ -2379,7 +2379,7 @@
       <c r="I46" t="s">
         <v>76</v>
       </c>
-      <c r="J46" s="95" t="s">
+      <c r="J46" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K46" t="s">
@@ -2388,7 +2388,7 @@
       <c r="L46" t="s">
         <v>79</v>
       </c>
-      <c r="Q46" s="102">
+      <c r="Q46" s="100">
         <v>2</v>
       </c>
     </row>
@@ -2411,7 +2411,7 @@
       <c r="I47" t="s">
         <v>76</v>
       </c>
-      <c r="J47" s="95" t="s">
+      <c r="J47" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K47" t="s">
@@ -2420,7 +2420,7 @@
       <c r="L47" t="s">
         <v>79</v>
       </c>
-      <c r="Q47" s="102">
+      <c r="Q47" s="100">
         <v>2</v>
       </c>
     </row>
@@ -2443,7 +2443,7 @@
       <c r="I48" t="s">
         <v>76</v>
       </c>
-      <c r="J48" s="95" t="s">
+      <c r="J48" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K48" t="s">
@@ -2452,7 +2452,7 @@
       <c r="L48" t="s">
         <v>79</v>
       </c>
-      <c r="Q48" s="102">
+      <c r="Q48" s="100">
         <v>2</v>
       </c>
     </row>
@@ -2475,7 +2475,7 @@
       <c r="I49" t="s">
         <v>76</v>
       </c>
-      <c r="J49" s="95" t="s">
+      <c r="J49" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K49" t="s">
@@ -2484,7 +2484,7 @@
       <c r="L49" t="s">
         <v>79</v>
       </c>
-      <c r="Q49" s="102">
+      <c r="Q49" s="100">
         <v>2</v>
       </c>
     </row>
@@ -2507,7 +2507,7 @@
       <c r="I50" t="s">
         <v>76</v>
       </c>
-      <c r="J50" s="95" t="s">
+      <c r="J50" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K50" t="s">
@@ -2516,7 +2516,7 @@
       <c r="L50" t="s">
         <v>79</v>
       </c>
-      <c r="Q50" s="102">
+      <c r="Q50" s="100">
         <v>2</v>
       </c>
     </row>
@@ -2528,7 +2528,7 @@
       </c>
       <c r="E51" s="9"/>
       <c r="F51" s="14"/>
-      <c r="Q51" s="102"/>
+      <c r="Q51" s="100"/>
     </row>
     <row r="52" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B52" s="16"/>
@@ -2549,7 +2549,7 @@
       <c r="I52" t="s">
         <v>76</v>
       </c>
-      <c r="J52" s="95" t="s">
+      <c r="J52" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K52" t="s">
@@ -2558,7 +2558,7 @@
       <c r="L52" t="s">
         <v>79</v>
       </c>
-      <c r="Q52" s="102">
+      <c r="Q52" s="100">
         <v>2</v>
       </c>
     </row>
@@ -2570,7 +2570,7 @@
       <c r="D53" s="20"/>
       <c r="E53" s="9"/>
       <c r="F53" s="14"/>
-      <c r="Q53" s="102"/>
+      <c r="Q53" s="100"/>
     </row>
     <row r="54" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B54" s="16"/>
@@ -2580,7 +2580,7 @@
       </c>
       <c r="E54" s="9"/>
       <c r="F54" s="14"/>
-      <c r="Q54" s="102"/>
+      <c r="Q54" s="100"/>
     </row>
     <row r="55" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B55" s="16"/>
@@ -2601,7 +2601,7 @@
       <c r="I55" t="s">
         <v>76</v>
       </c>
-      <c r="J55" s="95" t="s">
+      <c r="J55" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K55" t="s">
@@ -2610,7 +2610,7 @@
       <c r="L55" t="s">
         <v>79</v>
       </c>
-      <c r="Q55" s="102">
+      <c r="Q55" s="100">
         <v>2</v>
       </c>
     </row>
@@ -2633,7 +2633,7 @@
       <c r="I56" t="s">
         <v>76</v>
       </c>
-      <c r="J56" s="95" t="s">
+      <c r="J56" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K56" t="s">
@@ -2642,7 +2642,7 @@
       <c r="L56" t="s">
         <v>79</v>
       </c>
-      <c r="Q56" s="102">
+      <c r="Q56" s="100">
         <v>2</v>
       </c>
     </row>
@@ -2665,7 +2665,7 @@
       <c r="I57" t="s">
         <v>76</v>
       </c>
-      <c r="J57" s="95" t="s">
+      <c r="J57" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K57" t="s">
@@ -2674,7 +2674,7 @@
       <c r="L57" t="s">
         <v>79</v>
       </c>
-      <c r="Q57" s="102">
+      <c r="Q57" s="100">
         <v>2</v>
       </c>
     </row>
@@ -2697,7 +2697,7 @@
       <c r="I58" t="s">
         <v>76</v>
       </c>
-      <c r="J58" s="95" t="s">
+      <c r="J58" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K58" t="s">
@@ -2706,7 +2706,7 @@
       <c r="L58" t="s">
         <v>79</v>
       </c>
-      <c r="Q58" s="102">
+      <c r="Q58" s="100">
         <v>2</v>
       </c>
     </row>
@@ -2729,7 +2729,7 @@
       <c r="I59" t="s">
         <v>76</v>
       </c>
-      <c r="J59" s="95" t="s">
+      <c r="J59" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K59" t="s">
@@ -2738,7 +2738,7 @@
       <c r="L59" t="s">
         <v>79</v>
       </c>
-      <c r="Q59" s="102">
+      <c r="Q59" s="100">
         <v>2</v>
       </c>
     </row>
@@ -2750,7 +2750,7 @@
       </c>
       <c r="E60" s="9"/>
       <c r="F60" s="14"/>
-      <c r="Q60" s="102"/>
+      <c r="Q60" s="100"/>
     </row>
     <row r="61" spans="2:17" x14ac:dyDescent="0.4">
       <c r="B61" s="16"/>
@@ -2771,7 +2771,7 @@
       <c r="I61" t="s">
         <v>76</v>
       </c>
-      <c r="J61" s="95" t="s">
+      <c r="J61" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K61" t="s">
@@ -2780,7 +2780,7 @@
       <c r="L61" t="s">
         <v>79</v>
       </c>
-      <c r="Q61" s="102">
+      <c r="Q61" s="100">
         <v>2</v>
       </c>
     </row>
@@ -2803,7 +2803,7 @@
       <c r="I62" t="s">
         <v>76</v>
       </c>
-      <c r="J62" s="95" t="s">
+      <c r="J62" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K62" t="s">
@@ -2812,7 +2812,7 @@
       <c r="L62" t="s">
         <v>79</v>
       </c>
-      <c r="Q62" s="102">
+      <c r="Q62" s="100">
         <v>2</v>
       </c>
     </row>
@@ -2835,7 +2835,7 @@
       <c r="I63" t="s">
         <v>76</v>
       </c>
-      <c r="J63" s="95" t="s">
+      <c r="J63" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K63" t="s">
@@ -2844,7 +2844,7 @@
       <c r="L63" t="s">
         <v>79</v>
       </c>
-      <c r="Q63" s="102">
+      <c r="Q63" s="100">
         <v>2</v>
       </c>
     </row>
@@ -2856,7 +2856,7 @@
       </c>
       <c r="E64" s="9"/>
       <c r="F64" s="14"/>
-      <c r="Q64" s="102"/>
+      <c r="Q64" s="100"/>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B65" s="16"/>
@@ -2874,10 +2874,10 @@
       <c r="H65" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="I65" s="96" t="s">
-        <v>76</v>
-      </c>
-      <c r="J65" s="95" t="s">
+      <c r="I65" s="94" t="s">
+        <v>76</v>
+      </c>
+      <c r="J65" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K65" t="s">
@@ -2889,7 +2889,7 @@
       <c r="M65" t="s">
         <v>79</v>
       </c>
-      <c r="Q65" s="102">
+      <c r="Q65" s="100">
         <v>3</v>
       </c>
     </row>
@@ -2909,10 +2909,10 @@
       <c r="H66" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="I66" s="96" t="s">
-        <v>76</v>
-      </c>
-      <c r="J66" s="95" t="s">
+      <c r="I66" s="94" t="s">
+        <v>76</v>
+      </c>
+      <c r="J66" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K66" t="s">
@@ -2924,7 +2924,7 @@
       <c r="M66" t="s">
         <v>79</v>
       </c>
-      <c r="Q66" s="102">
+      <c r="Q66" s="100">
         <v>3</v>
       </c>
     </row>
@@ -2944,10 +2944,10 @@
       <c r="H67" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="I67" s="96" t="s">
-        <v>76</v>
-      </c>
-      <c r="J67" s="95" t="s">
+      <c r="I67" s="94" t="s">
+        <v>76</v>
+      </c>
+      <c r="J67" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K67" t="s">
@@ -2959,7 +2959,7 @@
       <c r="M67" t="s">
         <v>79</v>
       </c>
-      <c r="Q67" s="102">
+      <c r="Q67" s="100">
         <v>3</v>
       </c>
     </row>
@@ -2979,10 +2979,10 @@
       <c r="H68" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="I68" s="96" t="s">
-        <v>76</v>
-      </c>
-      <c r="J68" s="95" t="s">
+      <c r="I68" s="94" t="s">
+        <v>76</v>
+      </c>
+      <c r="J68" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K68" t="s">
@@ -2994,7 +2994,7 @@
       <c r="M68" t="s">
         <v>79</v>
       </c>
-      <c r="Q68" s="102">
+      <c r="Q68" s="100">
         <v>3</v>
       </c>
     </row>
@@ -3014,10 +3014,10 @@
       <c r="H69" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="I69" s="96" t="s">
-        <v>76</v>
-      </c>
-      <c r="J69" s="95" t="s">
+      <c r="I69" s="94" t="s">
+        <v>76</v>
+      </c>
+      <c r="J69" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K69" t="s">
@@ -3029,7 +3029,7 @@
       <c r="M69" t="s">
         <v>79</v>
       </c>
-      <c r="Q69" s="102">
+      <c r="Q69" s="100">
         <v>3</v>
       </c>
     </row>
@@ -3049,10 +3049,10 @@
       <c r="H70" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="I70" s="96" t="s">
-        <v>76</v>
-      </c>
-      <c r="J70" s="95" t="s">
+      <c r="I70" s="94" t="s">
+        <v>76</v>
+      </c>
+      <c r="J70" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K70" t="s">
@@ -3064,7 +3064,7 @@
       <c r="M70" t="s">
         <v>79</v>
       </c>
-      <c r="Q70" s="102">
+      <c r="Q70" s="100">
         <v>3</v>
       </c>
     </row>
@@ -3084,10 +3084,10 @@
       <c r="H71" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="I71" s="96" t="s">
-        <v>76</v>
-      </c>
-      <c r="J71" s="95" t="s">
+      <c r="I71" s="94" t="s">
+        <v>76</v>
+      </c>
+      <c r="J71" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K71" t="s">
@@ -3099,7 +3099,7 @@
       <c r="M71" t="s">
         <v>79</v>
       </c>
-      <c r="Q71" s="102">
+      <c r="Q71" s="100">
         <v>3</v>
       </c>
     </row>
@@ -3111,7 +3111,7 @@
       </c>
       <c r="E72" s="9"/>
       <c r="F72" s="14"/>
-      <c r="Q72" s="102"/>
+      <c r="Q72" s="100"/>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B73" s="16"/>
@@ -3129,10 +3129,10 @@
       <c r="H73" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="I73" s="96" t="s">
-        <v>76</v>
-      </c>
-      <c r="J73" s="95" t="s">
+      <c r="I73" s="94" t="s">
+        <v>76</v>
+      </c>
+      <c r="J73" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K73" t="s">
@@ -3144,7 +3144,7 @@
       <c r="M73" t="s">
         <v>79</v>
       </c>
-      <c r="Q73" s="102">
+      <c r="Q73" s="100">
         <v>3</v>
       </c>
     </row>
@@ -3164,10 +3164,10 @@
       <c r="H74" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="I74" s="96" t="s">
-        <v>76</v>
-      </c>
-      <c r="J74" s="95" t="s">
+      <c r="I74" s="94" t="s">
+        <v>76</v>
+      </c>
+      <c r="J74" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K74" t="s">
@@ -3179,14 +3179,14 @@
       <c r="M74" t="s">
         <v>79</v>
       </c>
-      <c r="Q74" s="102">
+      <c r="Q74" s="100">
         <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E75" s="7"/>
       <c r="F75" s="8"/>
-      <c r="Q75" s="102"/>
+      <c r="Q75" s="100"/>
     </row>
     <row r="76" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B76" s="28" t="s">
@@ -3196,7 +3196,7 @@
       <c r="D76" s="19"/>
       <c r="E76" s="12"/>
       <c r="F76" s="13"/>
-      <c r="Q76" s="102"/>
+      <c r="Q76" s="100"/>
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.4">
       <c r="B77" s="16"/>
@@ -3214,10 +3214,10 @@
       <c r="H77" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="I77" s="96" t="s">
-        <v>76</v>
-      </c>
-      <c r="J77" s="95" t="s">
+      <c r="I77" s="94" t="s">
+        <v>76</v>
+      </c>
+      <c r="J77" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K77" t="s">
@@ -3229,7 +3229,7 @@
       <c r="M77" t="s">
         <v>79</v>
       </c>
-      <c r="Q77" s="102">
+      <c r="Q77" s="100">
         <v>3</v>
       </c>
     </row>
@@ -3249,10 +3249,10 @@
       <c r="H78" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="I78" s="96" t="s">
-        <v>76</v>
-      </c>
-      <c r="J78" s="95" t="s">
+      <c r="I78" s="94" t="s">
+        <v>76</v>
+      </c>
+      <c r="J78" s="93" t="s">
         <v>80</v>
       </c>
       <c r="K78" t="s">
@@ -3264,7 +3264,7 @@
       <c r="M78" t="s">
         <v>79</v>
       </c>
-      <c r="Q78" s="104">
+      <c r="Q78" s="102">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update IFG-Penerimaan dan Pengeluaran.xlsx
add kode_sub for pengeluaran module
</commit_message>
<xml_diff>
--- a/Dokumen-si/IFG-Penerimaan dan Pengeluaran.xlsx
+++ b/Dokumen-si/IFG-Penerimaan dan Pengeluaran.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="105">
   <si>
     <t>kode</t>
   </si>
@@ -32,12 +32,6 @@
     <t>nama sub</t>
   </si>
   <si>
-    <t>PENDAPATAN TIDAK TERIKAT</t>
-  </si>
-  <si>
-    <t>Pendapatan Sewa</t>
-  </si>
-  <si>
     <t>Infaq peminjaman peralatan</t>
   </si>
   <si>
@@ -56,12 +50,6 @@
     <t>Pendapatan Lainnya</t>
   </si>
   <si>
-    <t>PENERIMAAN TERIKAT</t>
-  </si>
-  <si>
-    <t>Peribadatan</t>
-  </si>
-  <si>
     <t>Infaq Kotak Jumat</t>
   </si>
   <si>
@@ -80,9 +68,6 @@
     <t>Infaq TPA dan Tahfidz</t>
   </si>
   <si>
-    <t>ZIFWAF</t>
-  </si>
-  <si>
     <t>Infaq dari Donatur</t>
   </si>
   <si>
@@ -104,15 +89,6 @@
     <t>Waqaf</t>
   </si>
   <si>
-    <t>PENERIMAAN</t>
-  </si>
-  <si>
-    <t>PENGELUARAN</t>
-  </si>
-  <si>
-    <t>PEMBELIAN</t>
-  </si>
-  <si>
     <t>Pembelian Peralatan</t>
   </si>
   <si>
@@ -122,12 +98,6 @@
     <t>Pembelian Kendaraan</t>
   </si>
   <si>
-    <t>BEBAN</t>
-  </si>
-  <si>
-    <t>Beban Operrasional</t>
-  </si>
-  <si>
     <t>Beban Listrik, Air, dan Telepon</t>
   </si>
   <si>
@@ -152,12 +122,6 @@
     <t>Beban Lainnya</t>
   </si>
   <si>
-    <t>Beban Terikat</t>
-  </si>
-  <si>
-    <t>Beban Tidak Terikat</t>
-  </si>
-  <si>
     <t>Insentif Penceramah/Khatib</t>
   </si>
   <si>
@@ -173,9 +137,6 @@
     <t>Peribadatan Lainnya</t>
   </si>
   <si>
-    <t>Ramadhan</t>
-  </si>
-  <si>
     <t>Shalat Tarawih</t>
   </si>
   <si>
@@ -185,9 +146,6 @@
     <t>Peringatan Nuzulul Quran</t>
   </si>
   <si>
-    <t>Penyaluran Ziswaf</t>
-  </si>
-  <si>
     <t>Penyaluran Zakat Fitrah dan Fidyah</t>
   </si>
   <si>
@@ -215,9 +173,6 @@
     <t>Beban Pelatihan</t>
   </si>
   <si>
-    <t>RENOVASI DAN PEMBANGUNAN</t>
-  </si>
-  <si>
     <t>Pembelian Material</t>
   </si>
   <si>
@@ -272,24 +227,12 @@
     <t>Jenis</t>
   </si>
   <si>
-    <t>Nama Alat</t>
-  </si>
-  <si>
     <t>Merek</t>
   </si>
   <si>
     <t>Jumlah</t>
   </si>
   <si>
-    <t>Harga</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Jenis Kendaraan</t>
-  </si>
-  <si>
     <t>Nama Penerima</t>
   </si>
   <si>
@@ -306,6 +249,96 @@
   </si>
   <si>
     <t>Attribute</t>
+  </si>
+  <si>
+    <t>1.PENERIMAAN</t>
+  </si>
+  <si>
+    <t>1.PENDAPATAN TIDAK TERIKAT</t>
+  </si>
+  <si>
+    <t>1.Pendapatan Sewa</t>
+  </si>
+  <si>
+    <t>2.Pendapatan Parkir</t>
+  </si>
+  <si>
+    <t>3.Infaq Pengurusan Jenazah</t>
+  </si>
+  <si>
+    <t>4.Pendapatan non-halal</t>
+  </si>
+  <si>
+    <t>5.Pendapatan Lainnya</t>
+  </si>
+  <si>
+    <t>2.PENERIMAAN TERIKAT</t>
+  </si>
+  <si>
+    <t>6.Peribadatan</t>
+  </si>
+  <si>
+    <t>7.Pendidikan</t>
+  </si>
+  <si>
+    <t>8.ZIFWAF</t>
+  </si>
+  <si>
+    <t>2.PENGELUARAN</t>
+  </si>
+  <si>
+    <t>1.PEMBELIAN</t>
+  </si>
+  <si>
+    <t>2.BEBAN</t>
+  </si>
+  <si>
+    <t>1Beban Tidak Terikat</t>
+  </si>
+  <si>
+    <t>1.Beban Operrasional</t>
+  </si>
+  <si>
+    <t>2.Beban Lainnya</t>
+  </si>
+  <si>
+    <t>2.Beban Terikat</t>
+  </si>
+  <si>
+    <t>3.Peribadatan</t>
+  </si>
+  <si>
+    <t>4.Ramadhan</t>
+  </si>
+  <si>
+    <t>5.Penyaluran Ziswaf</t>
+  </si>
+  <si>
+    <t>6.Pendidikan</t>
+  </si>
+  <si>
+    <t>3.RENOVASI DAN PEMBANGUNAN</t>
+  </si>
+  <si>
+    <t>Harga Satuan</t>
+  </si>
+  <si>
+    <t>Total Harga</t>
+  </si>
+  <si>
+    <t>Nomor Seri</t>
+  </si>
+  <si>
+    <t>tr5_Renovasi</t>
+  </si>
+  <si>
+    <t>tr1_Penerimaan</t>
+  </si>
+  <si>
+    <t>tr2_pembelian</t>
+  </si>
+  <si>
+    <t>tr3_Beban1 &amp; tr4_Beban2</t>
   </si>
 </sst>
 </file>
@@ -531,7 +564,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -853,11 +886,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF00B0F0"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -977,6 +1019,15 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1292,10 +1343,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q85"/>
+  <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="K77" sqref="K77"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
@@ -1309,23 +1360,29 @@
     <col min="7" max="7" width="33.140625" style="47" customWidth="1"/>
     <col min="8" max="8" width="29.140625" style="42" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="17" max="17" width="24.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.7109375" customWidth="1"/>
+    <col min="19" max="19" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.4">
       <c r="E1" s="7"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
       <c r="E2" s="7"/>
       <c r="F2" s="8"/>
       <c r="G2" s="104" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="H2" s="104"/>
       <c r="I2" s="105" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="J2" s="105"/>
       <c r="K2" s="105"/>
@@ -1334,11 +1391,12 @@
       <c r="N2" s="105"/>
       <c r="O2" s="105"/>
       <c r="P2" s="105"/>
-      <c r="Q2" s="103" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="Q2" s="105"/>
+      <c r="R2" s="103" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A3" s="39"/>
       <c r="B3" s="24"/>
       <c r="C3" s="24"/>
@@ -1350,16 +1408,16 @@
         <v>1</v>
       </c>
       <c r="G3" s="48" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="H3" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q3" s="98"/>
-    </row>
-    <row r="4" spans="1:17" s="37" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+      <c r="R3" s="98"/>
+    </row>
+    <row r="4" spans="1:19" s="37" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A4" s="33" t="s">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="B4" s="34"/>
       <c r="C4" s="34"/>
@@ -1371,11 +1429,11 @@
       <c r="J4" s="91"/>
       <c r="K4" s="91"/>
       <c r="L4" s="91"/>
-      <c r="Q4" s="99"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R4" s="99"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B5" s="64" t="s">
-        <v>2</v>
+        <v>76</v>
       </c>
       <c r="C5" s="65"/>
       <c r="D5" s="66"/>
@@ -1385,15 +1443,18 @@
       <c r="J5" s="92"/>
       <c r="K5" s="92"/>
       <c r="L5" s="92"/>
-      <c r="Q5" s="100" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R5" s="100" t="s">
+        <v>72</v>
+      </c>
+      <c r="S5" s="107" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B6" s="69"/>
       <c r="C6" s="26"/>
       <c r="D6" s="53" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="E6" s="54"/>
       <c r="F6" s="70"/>
@@ -1403,77 +1464,80 @@
       <c r="J6" s="92"/>
       <c r="K6" s="92"/>
       <c r="L6" s="92"/>
-      <c r="Q6" s="100"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R6" s="100"/>
+      <c r="S6" s="107"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B7" s="69"/>
       <c r="C7" s="26"/>
       <c r="D7" s="56"/>
       <c r="E7" s="11">
-        <v>1111</v>
+        <v>11110</v>
       </c>
       <c r="F7" s="71" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="H7" s="62" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I7" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J7" s="96" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="K7" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L7" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q7" s="100">
+        <v>64</v>
+      </c>
+      <c r="R7" s="100">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S7" s="107"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B8" s="69"/>
       <c r="C8" s="26"/>
       <c r="D8" s="57"/>
       <c r="E8" s="58">
-        <v>1112</v>
+        <v>11120</v>
       </c>
       <c r="F8" s="72" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G8" s="95" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="H8" s="63" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I8" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J8" s="96" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="K8" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L8" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q8" s="100">
+        <v>64</v>
+      </c>
+      <c r="R8" s="100">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S8" s="107"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B9" s="69"/>
       <c r="C9" s="26"/>
       <c r="D9" s="53" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="E9" s="54"/>
       <c r="F9" s="70"/>
@@ -1483,43 +1547,45 @@
       <c r="J9" s="92"/>
       <c r="K9" s="92"/>
       <c r="L9" s="92"/>
-      <c r="Q9" s="100"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R9" s="100"/>
+      <c r="S9" s="107"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B10" s="69"/>
       <c r="C10" s="26"/>
       <c r="D10" s="57"/>
       <c r="E10" s="58">
-        <v>1120</v>
+        <v>11200</v>
       </c>
       <c r="F10" s="73" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G10" s="95" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="H10" s="63" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I10" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J10" s="97"/>
       <c r="K10" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L10" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q10" s="100">
+        <v>64</v>
+      </c>
+      <c r="R10" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S10" s="107"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B11" s="69"/>
       <c r="C11" s="26"/>
       <c r="D11" s="59" t="s">
-        <v>7</v>
+        <v>79</v>
       </c>
       <c r="E11" s="54"/>
       <c r="F11" s="70"/>
@@ -1529,45 +1595,47 @@
       <c r="J11" s="10"/>
       <c r="K11" s="92"/>
       <c r="L11" s="92"/>
-      <c r="Q11" s="100"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R11" s="100"/>
+      <c r="S11" s="107"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B12" s="69"/>
       <c r="C12" s="26"/>
       <c r="D12" s="57"/>
       <c r="E12" s="58">
-        <v>1130</v>
+        <v>11300</v>
       </c>
       <c r="F12" s="73" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G12" s="95" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="H12" s="63" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="I12" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J12" s="96" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="K12" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L12" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q12" s="100">
+        <v>64</v>
+      </c>
+      <c r="R12" s="100">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S12" s="107"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B13" s="69"/>
       <c r="C13" s="26"/>
       <c r="D13" s="59" t="s">
-        <v>8</v>
+        <v>80</v>
       </c>
       <c r="E13" s="54"/>
       <c r="F13" s="70"/>
@@ -1577,45 +1645,47 @@
       <c r="J13" s="10"/>
       <c r="K13" s="92"/>
       <c r="L13" s="92"/>
-      <c r="Q13" s="100"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R13" s="100"/>
+      <c r="S13" s="107"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B14" s="69"/>
       <c r="C14" s="26"/>
       <c r="D14" s="57"/>
       <c r="E14" s="58">
-        <v>1140</v>
+        <v>11400</v>
       </c>
       <c r="F14" s="73" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G14" s="95" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="H14" s="63" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I14" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J14" s="96" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="K14" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L14" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q14" s="100">
+        <v>64</v>
+      </c>
+      <c r="R14" s="100">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S14" s="107"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B15" s="69"/>
       <c r="C15" s="26"/>
       <c r="D15" s="60" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="E15" s="54"/>
       <c r="F15" s="70"/>
@@ -1625,50 +1695,53 @@
       <c r="J15" s="10"/>
       <c r="K15" s="92"/>
       <c r="L15" s="92"/>
-      <c r="Q15" s="100"/>
-    </row>
-    <row r="16" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="R15" s="100"/>
+      <c r="S15" s="107"/>
+    </row>
+    <row r="16" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B16" s="74"/>
       <c r="C16" s="75"/>
       <c r="D16" s="57"/>
       <c r="E16" s="58">
-        <v>1150</v>
+        <v>11500</v>
       </c>
       <c r="F16" s="73" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G16" s="78" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="H16" s="63" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="I16" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J16" s="97"/>
       <c r="K16" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L16" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q16" s="100">
+        <v>64</v>
+      </c>
+      <c r="R16" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="2:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="S16" s="107"/>
+    </row>
+    <row r="17" spans="2:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E17" s="7"/>
       <c r="F17" s="8"/>
       <c r="I17" s="92"/>
       <c r="J17" s="10"/>
       <c r="K17" s="92"/>
       <c r="L17" s="92"/>
-      <c r="Q17" s="100"/>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="R17" s="100"/>
+      <c r="S17" s="107"/>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B18" s="76" t="s">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="C18" s="77"/>
       <c r="D18" s="66"/>
@@ -1678,13 +1751,14 @@
       <c r="J18" s="10"/>
       <c r="K18" s="92"/>
       <c r="L18" s="92"/>
-      <c r="Q18" s="100"/>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="R18" s="100"/>
+      <c r="S18" s="107"/>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B19" s="69"/>
       <c r="C19" s="26"/>
       <c r="D19" s="59" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="E19" s="54"/>
       <c r="F19" s="70"/>
@@ -1694,133 +1768,138 @@
       <c r="J19" s="10"/>
       <c r="K19" s="92"/>
       <c r="L19" s="92"/>
-      <c r="Q19" s="100"/>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="R19" s="100"/>
+      <c r="S19" s="107"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B20" s="69"/>
       <c r="C20" s="26"/>
       <c r="D20" s="56"/>
       <c r="E20" s="11">
-        <v>1261</v>
+        <v>12610</v>
       </c>
       <c r="F20" s="71" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G20" s="52" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="H20" s="62" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I20" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J20" s="97"/>
       <c r="K20" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L20" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q20" s="100">
+        <v>64</v>
+      </c>
+      <c r="R20" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S20" s="107"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B21" s="69"/>
       <c r="C21" s="26"/>
       <c r="D21" s="56"/>
       <c r="E21" s="11">
-        <v>1262</v>
+        <v>12620</v>
       </c>
       <c r="F21" s="71" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G21" s="52" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="H21" s="62" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I21" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J21" s="97"/>
       <c r="K21" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L21" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q21" s="100">
+        <v>64</v>
+      </c>
+      <c r="R21" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S21" s="107"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B22" s="69"/>
       <c r="C22" s="26"/>
       <c r="D22" s="56"/>
       <c r="E22" s="11">
-        <v>1263</v>
+        <v>12630</v>
       </c>
       <c r="F22" s="71" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G22" s="52" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="H22" s="62" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I22" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J22" s="97"/>
       <c r="K22" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L22" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q22" s="100">
+        <v>64</v>
+      </c>
+      <c r="R22" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S22" s="107"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B23" s="69"/>
       <c r="C23" s="26"/>
       <c r="D23" s="57"/>
-      <c r="E23" s="58">
-        <v>1264</v>
+      <c r="E23" s="11">
+        <v>12640</v>
       </c>
       <c r="F23" s="73" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G23" s="95" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="H23" s="63" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="I23" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J23" s="97"/>
       <c r="K23" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L23" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q23" s="100">
+        <v>64</v>
+      </c>
+      <c r="R23" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S23" s="107"/>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B24" s="69"/>
       <c r="C24" s="26"/>
       <c r="D24" s="59" t="s">
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="E24" s="54"/>
       <c r="F24" s="70"/>
@@ -1830,45 +1909,47 @@
       <c r="J24" s="92"/>
       <c r="K24" s="92"/>
       <c r="L24" s="92"/>
-      <c r="Q24" s="100"/>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="R24" s="100"/>
+      <c r="S24" s="107"/>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B25" s="69"/>
       <c r="C25" s="26"/>
       <c r="D25" s="57"/>
       <c r="E25" s="58">
-        <v>1270</v>
+        <v>12700</v>
       </c>
       <c r="F25" s="73" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G25" s="95" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="H25" s="63" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="I25" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J25" s="96" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="K25" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L25" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q25" s="100">
+        <v>64</v>
+      </c>
+      <c r="R25" s="100">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S25" s="107"/>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B26" s="69"/>
       <c r="C26" s="26"/>
       <c r="D26" s="59" t="s">
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="E26" s="54"/>
       <c r="F26" s="70"/>
@@ -1878,238 +1959,247 @@
       <c r="J26" s="92"/>
       <c r="K26" s="92"/>
       <c r="L26" s="92"/>
-      <c r="Q26" s="100"/>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="R26" s="100"/>
+      <c r="S26" s="107"/>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B27" s="69"/>
       <c r="C27" s="26"/>
       <c r="D27" s="56"/>
       <c r="E27" s="11">
-        <v>1281</v>
+        <v>12810</v>
       </c>
       <c r="F27" s="71" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G27" s="52" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="H27" s="62" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I27" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J27" s="96" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="K27" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L27" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q27" s="100">
+        <v>64</v>
+      </c>
+      <c r="R27" s="100">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S27" s="107"/>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B28" s="69"/>
       <c r="C28" s="26"/>
       <c r="D28" s="56"/>
       <c r="E28" s="11">
-        <v>1282</v>
+        <v>12820</v>
       </c>
       <c r="F28" s="71" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="G28" s="52" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="H28" s="62" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="I28" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J28" s="97"/>
       <c r="K28" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L28" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q28" s="100">
+        <v>64</v>
+      </c>
+      <c r="R28" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S28" s="107"/>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B29" s="69"/>
       <c r="C29" s="26"/>
       <c r="D29" s="56"/>
       <c r="E29" s="11">
-        <v>1283</v>
+        <v>12830</v>
       </c>
       <c r="F29" s="71" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="G29" s="52" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="H29" s="62" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="I29" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J29" s="96" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="K29" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L29" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q29" s="100">
+        <v>64</v>
+      </c>
+      <c r="R29" s="100">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S29" s="107"/>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B30" s="69"/>
       <c r="C30" s="26"/>
       <c r="D30" s="56"/>
       <c r="E30" s="11">
-        <v>1284</v>
+        <v>12840</v>
       </c>
       <c r="F30" s="71" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G30" s="52" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="H30" s="62" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I30" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J30" s="96" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="K30" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L30" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q30" s="100">
+        <v>64</v>
+      </c>
+      <c r="R30" s="100">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S30" s="107"/>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B31" s="69"/>
       <c r="C31" s="26"/>
       <c r="D31" s="56"/>
       <c r="E31" s="11">
-        <v>1285</v>
+        <v>12850</v>
       </c>
       <c r="F31" s="71" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="G31" s="52" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="H31" s="62" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="I31" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J31" s="96" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="K31" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L31" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q31" s="100">
+        <v>64</v>
+      </c>
+      <c r="R31" s="100">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S31" s="107"/>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B32" s="69"/>
       <c r="C32" s="26"/>
       <c r="D32" s="56"/>
       <c r="E32" s="11">
-        <v>1286</v>
+        <v>12860</v>
       </c>
       <c r="F32" s="71" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G32" s="52" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="H32" s="62" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="I32" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J32" s="96" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="K32" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L32" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q32" s="100">
+        <v>64</v>
+      </c>
+      <c r="R32" s="100">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="S32" s="107"/>
+    </row>
+    <row r="33" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B33" s="74"/>
       <c r="C33" s="75"/>
       <c r="D33" s="57"/>
       <c r="E33" s="58">
-        <v>1287</v>
+        <v>12870</v>
       </c>
       <c r="F33" s="73" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G33" s="78" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="H33" s="63" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="I33" s="96" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J33" s="96" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="K33" s="96" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L33" s="96" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q33" s="100">
+        <v>64</v>
+      </c>
+      <c r="R33" s="100">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S33" s="107"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.4">
       <c r="E34" s="7"/>
       <c r="F34" s="8"/>
-      <c r="Q34" s="100"/>
-    </row>
-    <row r="35" spans="1:17" s="2" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="R34" s="100"/>
+      <c r="S34" s="107"/>
+    </row>
+    <row r="35" spans="1:19" s="2" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A35" s="33" t="s">
-        <v>27</v>
+        <v>86</v>
       </c>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
@@ -2117,186 +2207,193 @@
       <c r="E35" s="32"/>
       <c r="G35" s="50"/>
       <c r="H35" s="45"/>
-      <c r="Q35" s="101"/>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R35" s="101"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B36" s="28" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
       <c r="C36" s="29"/>
       <c r="D36" s="19"/>
       <c r="E36" s="12"/>
       <c r="F36" s="13"/>
-      <c r="Q36" s="100" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R36" s="100" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B37" s="16"/>
       <c r="C37" s="26"/>
       <c r="D37" s="20"/>
       <c r="E37" s="11">
-        <v>2110</v>
+        <v>21100</v>
       </c>
       <c r="F37" s="79" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G37" s="81" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="H37" s="82" t="s">
+        <v>51</v>
+      </c>
+      <c r="I37" t="s">
+        <v>61</v>
+      </c>
+      <c r="J37" t="s">
         <v>66</v>
       </c>
-      <c r="I37" t="s">
-        <v>76</v>
-      </c>
-      <c r="J37" s="93" t="s">
-        <v>80</v>
-      </c>
       <c r="K37" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="L37" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="M37" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="N37" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="O37" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="P37" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q37" s="100">
+        <v>99</v>
+      </c>
+      <c r="R37" s="100">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S37" s="108" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B38" s="16"/>
       <c r="C38" s="26"/>
       <c r="D38" s="20"/>
       <c r="E38" s="11">
-        <v>2120</v>
+        <v>21200</v>
       </c>
       <c r="F38" s="79" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G38" s="83" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="H38" s="84" t="s">
+        <v>51</v>
+      </c>
+      <c r="I38" t="s">
+        <v>61</v>
+      </c>
+      <c r="J38" t="s">
         <v>66</v>
       </c>
-      <c r="I38" t="s">
-        <v>76</v>
-      </c>
-      <c r="J38" s="93" t="s">
-        <v>80</v>
-      </c>
       <c r="K38" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="L38" t="s">
-        <v>82</v>
+        <v>100</v>
       </c>
       <c r="M38" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="N38" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="O38" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="P38" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q38" s="100">
+        <v>99</v>
+      </c>
+      <c r="R38" s="100">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="S38" s="108"/>
+    </row>
+    <row r="39" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B39" s="25"/>
       <c r="C39" s="27"/>
       <c r="D39" s="21"/>
       <c r="E39" s="15">
-        <v>2130</v>
+        <v>21300</v>
       </c>
       <c r="F39" s="80" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G39" s="85" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="H39" s="86" t="s">
+        <v>51</v>
+      </c>
+      <c r="I39" t="s">
+        <v>61</v>
+      </c>
+      <c r="J39" s="93" t="s">
         <v>66</v>
       </c>
-      <c r="I39" t="s">
-        <v>76</v>
-      </c>
-      <c r="J39" s="93" t="s">
-        <v>80</v>
-      </c>
-      <c r="K39" s="93" t="s">
-        <v>87</v>
-      </c>
-      <c r="L39" s="2"/>
+      <c r="K39" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="L39" t="s">
+        <v>100</v>
+      </c>
       <c r="M39" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="N39" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="O39" t="s">
-        <v>85</v>
+        <v>98</v>
       </c>
       <c r="P39" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q39" s="100">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+        <v>99</v>
+      </c>
+      <c r="R39" s="100">
+        <v>1</v>
+      </c>
+      <c r="S39" s="108"/>
+    </row>
+    <row r="40" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E40" s="7"/>
       <c r="F40" s="8"/>
-      <c r="Q40" s="100"/>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R40" s="100"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B41" s="28" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="C41" s="29"/>
       <c r="D41" s="19"/>
       <c r="E41" s="12"/>
       <c r="F41" s="13"/>
-      <c r="Q41" s="100"/>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R41" s="100"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B42" s="16"/>
       <c r="C42" s="26" t="s">
-        <v>43</v>
+        <v>89</v>
       </c>
       <c r="D42" s="20"/>
       <c r="E42" s="9"/>
       <c r="F42" s="14"/>
-      <c r="Q42" s="100"/>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R42" s="100"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B43" s="16"/>
       <c r="C43" s="26"/>
       <c r="D43" s="20" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="E43" s="9"/>
       <c r="F43" s="14"/>
-      <c r="Q43" s="100"/>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R43" s="100"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B44" s="16"/>
       <c r="C44" s="26"/>
       <c r="D44" s="20"/>
@@ -2304,971 +2401,1005 @@
         <v>22111</v>
       </c>
       <c r="F44" s="79" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="G44" s="87" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="H44" s="82" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I44" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J44" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K44" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L44" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q44" s="100">
+        <v>64</v>
+      </c>
+      <c r="R44" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S44" s="106" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B45" s="16"/>
       <c r="C45" s="26"/>
       <c r="D45" s="20"/>
       <c r="E45" s="11">
-        <v>502</v>
+        <v>22112</v>
       </c>
       <c r="F45" s="79" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="G45" s="88" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="H45" s="84" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I45" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J45" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K45" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L45" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q45" s="100">
+        <v>64</v>
+      </c>
+      <c r="R45" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S45" s="106"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B46" s="16"/>
       <c r="C46" s="26"/>
       <c r="D46" s="20"/>
       <c r="E46" s="11">
-        <v>503</v>
+        <v>22113</v>
       </c>
       <c r="F46" s="79" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="G46" s="88" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="H46" s="84" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I46" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J46" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K46" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L46" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q46" s="100">
+        <v>64</v>
+      </c>
+      <c r="R46" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S46" s="106"/>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B47" s="16"/>
       <c r="C47" s="26"/>
       <c r="D47" s="20"/>
       <c r="E47" s="11">
-        <v>504</v>
+        <v>22114</v>
       </c>
       <c r="F47" s="79" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="G47" s="88" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="H47" s="84" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I47" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J47" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K47" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L47" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q47" s="100">
+        <v>64</v>
+      </c>
+      <c r="R47" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S47" s="106"/>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B48" s="16"/>
       <c r="C48" s="26"/>
       <c r="D48" s="20"/>
       <c r="E48" s="11">
-        <v>505</v>
+        <v>22115</v>
       </c>
       <c r="F48" s="79" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="G48" s="88" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="H48" s="84" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I48" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J48" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K48" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L48" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q48" s="100">
+        <v>64</v>
+      </c>
+      <c r="R48" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S48" s="106"/>
+    </row>
+    <row r="49" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B49" s="16"/>
       <c r="C49" s="26"/>
       <c r="D49" s="20"/>
       <c r="E49" s="11">
-        <v>506</v>
+        <v>22116</v>
       </c>
       <c r="F49" s="79" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="G49" s="88" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="H49" s="84" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I49" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J49" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K49" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L49" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q49" s="100">
+        <v>64</v>
+      </c>
+      <c r="R49" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S49" s="106"/>
+    </row>
+    <row r="50" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B50" s="16"/>
       <c r="C50" s="26"/>
       <c r="D50" s="20"/>
       <c r="E50" s="11">
-        <v>507</v>
+        <v>22117</v>
       </c>
       <c r="F50" s="79" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G50" s="85" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H50" s="86" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I50" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J50" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K50" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L50" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q50" s="100">
+        <v>64</v>
+      </c>
+      <c r="R50" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S50" s="106"/>
+    </row>
+    <row r="51" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B51" s="16"/>
       <c r="C51" s="26"/>
       <c r="D51" s="20" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="E51" s="9"/>
       <c r="F51" s="14"/>
-      <c r="Q51" s="100"/>
-    </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="R51" s="100"/>
+      <c r="S51" s="106"/>
+    </row>
+    <row r="52" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B52" s="16"/>
       <c r="C52" s="26"/>
       <c r="D52" s="20"/>
       <c r="E52" s="11">
-        <v>559</v>
+        <v>22120</v>
       </c>
       <c r="F52" s="79" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="G52" s="89" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="H52" s="90" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I52" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J52" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K52" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L52" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q52" s="100">
+        <v>64</v>
+      </c>
+      <c r="R52" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S52" s="106"/>
+    </row>
+    <row r="53" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B53" s="16"/>
       <c r="C53" s="26" t="s">
-        <v>42</v>
+        <v>92</v>
       </c>
       <c r="D53" s="20"/>
       <c r="E53" s="9"/>
       <c r="F53" s="14"/>
-      <c r="Q53" s="100"/>
-    </row>
-    <row r="54" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="R53" s="100"/>
+      <c r="S53" s="106"/>
+    </row>
+    <row r="54" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B54" s="16"/>
       <c r="C54" s="26"/>
       <c r="D54" s="20" t="s">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="E54" s="9"/>
       <c r="F54" s="14"/>
-      <c r="Q54" s="100"/>
-    </row>
-    <row r="55" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="R54" s="100"/>
+      <c r="S54" s="106"/>
+    </row>
+    <row r="55" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B55" s="16"/>
       <c r="C55" s="26"/>
       <c r="D55" s="20"/>
       <c r="E55" s="11">
-        <v>521</v>
+        <v>22231</v>
       </c>
       <c r="F55" s="79" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="G55" s="87" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="H55" s="61" t="s">
-        <v>66</v>
-      </c>
-      <c r="I55" t="s">
-        <v>76</v>
+        <v>51</v>
+      </c>
+      <c r="I55" s="94" t="s">
+        <v>61</v>
       </c>
       <c r="J55" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K55" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="L55" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q55" s="100">
+        <v>63</v>
+      </c>
+      <c r="M55" t="s">
+        <v>64</v>
+      </c>
+      <c r="R55" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S55" s="106"/>
+    </row>
+    <row r="56" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B56" s="16"/>
       <c r="C56" s="26"/>
       <c r="D56" s="20"/>
       <c r="E56" s="11">
-        <v>522</v>
+        <v>22232</v>
       </c>
       <c r="F56" s="79" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="G56" s="88" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="H56" s="62" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I56" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J56" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K56" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L56" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q56" s="100">
+        <v>64</v>
+      </c>
+      <c r="R56" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S56" s="106"/>
+    </row>
+    <row r="57" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B57" s="16"/>
       <c r="C57" s="26"/>
       <c r="D57" s="20"/>
       <c r="E57" s="11">
-        <v>523</v>
+        <v>22233</v>
       </c>
       <c r="F57" s="79" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="G57" s="88" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="H57" s="62" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I57" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J57" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K57" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L57" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q57" s="100">
+        <v>64</v>
+      </c>
+      <c r="R57" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S57" s="106"/>
+    </row>
+    <row r="58" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B58" s="16"/>
       <c r="C58" s="26"/>
       <c r="D58" s="20"/>
       <c r="E58" s="11">
-        <v>524</v>
+        <v>22234</v>
       </c>
       <c r="F58" s="79" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="G58" s="88" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="H58" s="62" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I58" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J58" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K58" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L58" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q58" s="100">
+        <v>64</v>
+      </c>
+      <c r="R58" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S58" s="106"/>
+    </row>
+    <row r="59" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B59" s="16"/>
       <c r="C59" s="26"/>
       <c r="D59" s="20"/>
       <c r="E59" s="11">
-        <v>525</v>
+        <v>22235</v>
       </c>
       <c r="F59" s="79" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G59" s="85" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="H59" s="63" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I59" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J59" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K59" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L59" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q59" s="100">
+        <v>64</v>
+      </c>
+      <c r="R59" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S59" s="106"/>
+    </row>
+    <row r="60" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B60" s="16"/>
       <c r="C60" s="26"/>
       <c r="D60" s="20" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="E60" s="9"/>
       <c r="F60" s="14"/>
-      <c r="Q60" s="100"/>
-    </row>
-    <row r="61" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="R60" s="100"/>
+      <c r="S60" s="106"/>
+    </row>
+    <row r="61" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B61" s="16"/>
       <c r="C61" s="26"/>
       <c r="D61" s="20"/>
       <c r="E61" s="11">
-        <v>531</v>
+        <v>22241</v>
       </c>
       <c r="F61" s="79" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="G61" s="87" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="H61" s="61" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I61" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J61" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K61" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L61" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q61" s="100">
+        <v>64</v>
+      </c>
+      <c r="R61" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S61" s="106"/>
+    </row>
+    <row r="62" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B62" s="16"/>
       <c r="C62" s="26"/>
       <c r="D62" s="20"/>
       <c r="E62" s="11">
-        <v>532</v>
+        <v>22242</v>
       </c>
       <c r="F62" s="79" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="G62" s="88" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="H62" s="62" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I62" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J62" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K62" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L62" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q62" s="100">
+        <v>64</v>
+      </c>
+      <c r="R62" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S62" s="106"/>
+    </row>
+    <row r="63" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B63" s="16"/>
       <c r="C63" s="26"/>
       <c r="D63" s="20"/>
       <c r="E63" s="11">
-        <v>533</v>
+        <v>22243</v>
       </c>
       <c r="F63" s="79" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="G63" s="85" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="H63" s="63" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I63" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J63" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K63" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="L63" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q63" s="100">
+        <v>64</v>
+      </c>
+      <c r="R63" s="100">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="S63" s="106"/>
+    </row>
+    <row r="64" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B64" s="16"/>
       <c r="C64" s="26"/>
       <c r="D64" s="20" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="E64" s="9"/>
       <c r="F64" s="14"/>
-      <c r="Q64" s="100"/>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R64" s="100"/>
+      <c r="S64" s="106"/>
+    </row>
+    <row r="65" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B65" s="16"/>
       <c r="C65" s="26"/>
       <c r="D65" s="20"/>
       <c r="E65" s="11">
-        <v>541</v>
+        <v>22251</v>
       </c>
       <c r="F65" s="79" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="G65" s="87" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="H65" s="61" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I65" s="94" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J65" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K65" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="L65" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="M65" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q65" s="100">
+        <v>64</v>
+      </c>
+      <c r="R65" s="100">
         <v>3</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S65" s="106"/>
+    </row>
+    <row r="66" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B66" s="16"/>
       <c r="C66" s="26"/>
       <c r="D66" s="20"/>
       <c r="E66" s="11">
-        <v>542</v>
+        <v>22252</v>
       </c>
       <c r="F66" s="79" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="G66" s="88" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="H66" s="62" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I66" s="94" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J66" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K66" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="L66" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="M66" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q66" s="100">
+        <v>64</v>
+      </c>
+      <c r="R66" s="100">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S66" s="106"/>
+    </row>
+    <row r="67" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B67" s="16"/>
       <c r="C67" s="26"/>
       <c r="D67" s="20"/>
       <c r="E67" s="11">
-        <v>543</v>
+        <v>22253</v>
       </c>
       <c r="F67" s="79" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="G67" s="88" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="H67" s="62" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I67" s="94" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J67" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K67" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="L67" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="M67" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q67" s="100">
+        <v>64</v>
+      </c>
+      <c r="R67" s="100">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S67" s="106"/>
+    </row>
+    <row r="68" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B68" s="16"/>
       <c r="C68" s="26"/>
       <c r="D68" s="20"/>
       <c r="E68" s="11">
-        <v>544</v>
+        <v>22254</v>
       </c>
       <c r="F68" s="79" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="G68" s="88" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="H68" s="62" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I68" s="94" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J68" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K68" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="L68" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="M68" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q68" s="100">
+        <v>64</v>
+      </c>
+      <c r="R68" s="100">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S68" s="106"/>
+    </row>
+    <row r="69" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B69" s="16"/>
       <c r="C69" s="26"/>
       <c r="D69" s="20"/>
       <c r="E69" s="11">
-        <v>545</v>
+        <v>22255</v>
       </c>
       <c r="F69" s="79" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="G69" s="88" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="H69" s="62" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I69" s="94" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J69" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K69" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="L69" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="M69" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q69" s="100">
+        <v>64</v>
+      </c>
+      <c r="R69" s="100">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S69" s="106"/>
+    </row>
+    <row r="70" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B70" s="16"/>
       <c r="C70" s="26"/>
       <c r="D70" s="20"/>
       <c r="E70" s="11">
-        <v>546</v>
+        <v>22256</v>
       </c>
       <c r="F70" s="79" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="G70" s="88" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="H70" s="62" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I70" s="94" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J70" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K70" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="L70" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="M70" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q70" s="100">
+        <v>64</v>
+      </c>
+      <c r="R70" s="100">
         <v>3</v>
       </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S70" s="106"/>
+    </row>
+    <row r="71" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B71" s="16"/>
       <c r="C71" s="26"/>
       <c r="D71" s="20"/>
       <c r="E71" s="11">
-        <v>547</v>
+        <v>22257</v>
       </c>
       <c r="F71" s="79" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="G71" s="85" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="H71" s="63" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I71" s="94" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J71" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K71" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="L71" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="M71" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q71" s="100">
+        <v>64</v>
+      </c>
+      <c r="R71" s="100">
         <v>3</v>
       </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="S71" s="106"/>
+    </row>
+    <row r="72" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B72" s="16"/>
       <c r="C72" s="26"/>
       <c r="D72" s="20" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="E72" s="9"/>
       <c r="F72" s="14"/>
-      <c r="Q72" s="100"/>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R72" s="100"/>
+      <c r="S72" s="106"/>
+    </row>
+    <row r="73" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B73" s="16"/>
       <c r="C73" s="26"/>
       <c r="D73" s="20"/>
       <c r="E73" s="11">
-        <v>551</v>
+        <v>22261</v>
       </c>
       <c r="F73" s="79" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="G73" s="87" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="H73" s="61" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I73" s="94" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J73" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K73" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="L73" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="M73" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q73" s="100">
+        <v>64</v>
+      </c>
+      <c r="R73" s="100">
         <v>3</v>
       </c>
-    </row>
-    <row r="74" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="S73" s="106"/>
+    </row>
+    <row r="74" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B74" s="25"/>
       <c r="C74" s="27"/>
       <c r="D74" s="21"/>
       <c r="E74" s="15">
-        <v>552</v>
+        <v>22262</v>
       </c>
       <c r="F74" s="80" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="G74" s="85" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="H74" s="63" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I74" s="94" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="J74" s="93" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="K74" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="L74" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="M74" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q74" s="100">
+        <v>64</v>
+      </c>
+      <c r="R74" s="100">
         <v>3</v>
       </c>
-    </row>
-    <row r="75" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="S74" s="106"/>
+    </row>
+    <row r="75" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="E75" s="7"/>
       <c r="F75" s="8"/>
-      <c r="Q75" s="100"/>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R75" s="100"/>
+    </row>
+    <row r="76" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B76" s="28" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="C76" s="29"/>
       <c r="D76" s="19"/>
       <c r="E76" s="12"/>
       <c r="F76" s="13"/>
-      <c r="Q76" s="100"/>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.4">
+      <c r="R76" s="100"/>
+    </row>
+    <row r="77" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B77" s="16"/>
       <c r="C77" s="26"/>
       <c r="D77" s="20"/>
       <c r="E77" s="11">
-        <v>511</v>
+        <v>23100</v>
       </c>
       <c r="F77" s="79" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="G77" s="87" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="H77" s="61" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I77" s="94" t="s">
-        <v>76</v>
-      </c>
-      <c r="J77" s="93" t="s">
-        <v>80</v>
+        <v>61</v>
+      </c>
+      <c r="J77" t="s">
+        <v>69</v>
       </c>
       <c r="K77" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="L77" t="s">
-        <v>78</v>
-      </c>
-      <c r="M77" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q77" s="100">
+        <v>64</v>
+      </c>
+      <c r="R77" s="100">
         <v>3</v>
       </c>
-    </row>
-    <row r="78" spans="1:17" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="S77" s="106" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="78" spans="1:19" ht="20.25" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B78" s="25"/>
       <c r="C78" s="27"/>
       <c r="D78" s="21"/>
       <c r="E78" s="15">
-        <v>512</v>
+        <v>23200</v>
       </c>
       <c r="F78" s="80" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="G78" s="85" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="H78" s="63" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="I78" s="94" t="s">
-        <v>76</v>
-      </c>
-      <c r="J78" s="93" t="s">
-        <v>80</v>
+        <v>61</v>
+      </c>
+      <c r="J78" t="s">
+        <v>69</v>
       </c>
       <c r="K78" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="L78" t="s">
-        <v>78</v>
-      </c>
-      <c r="M78" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q78" s="102">
+        <v>64</v>
+      </c>
+      <c r="R78" s="102">
         <v>3</v>
       </c>
-    </row>
-    <row r="79" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="S78" s="106"/>
+    </row>
+    <row r="79" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A79" s="40"/>
       <c r="B79" s="41"/>
       <c r="C79" s="41"/>
@@ -3278,7 +3409,7 @@
       <c r="G79" s="51"/>
       <c r="H79" s="46"/>
     </row>
-    <row r="80" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:19" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A80" s="40"/>
       <c r="B80" s="41"/>
       <c r="C80" s="41"/>
@@ -3327,9 +3458,13 @@
       <c r="H85"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="S77:S78"/>
     <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:P2"/>
+    <mergeCell ref="I2:Q2"/>
+    <mergeCell ref="S37:S39"/>
+    <mergeCell ref="S5:S34"/>
+    <mergeCell ref="S44:S74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>